<commit_message>
clean up and minor changes
</commit_message>
<xml_diff>
--- a/01_Data/Femizide/femizide_Schweiz_raw.xlsx
+++ b/01_Data/Femizide/femizide_Schweiz_raw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LucaK\OneDrive\Desktop\GitHub\Femizide_Schweiz\01_Data\Femizide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66635FA3-1A6A-431B-B27B-C58EB69A249A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{223FC273-A46F-4FCD-9A7C-8EEB2AA2E55D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19875" yWindow="4125" windowWidth="23040" windowHeight="13560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="29010" windowHeight="23385" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="301">
   <si>
     <t>rowid</t>
   </si>
@@ -725,15 +725,6 @@
     <t>Die Frau überlebt. Sie ist 52 Jahre alt.</t>
   </si>
   <si>
-    <t>Sie ist 29 Jahre alt.</t>
-  </si>
-  <si>
-    <t>Sie ist 45 Jahre alt.</t>
-  </si>
-  <si>
-    <t>Sie ist 48 Jahre alt.</t>
-  </si>
-  <si>
     <t>Kehrsatz</t>
   </si>
   <si>
@@ -782,9 +773,6 @@
     <t>Hamburg, Deutschland. Ein 22-jähriger Schweizer tötet eine Frau.</t>
   </si>
   <si>
-    <t>Die Frau wurde 22 Jahre alt.</t>
-  </si>
-  <si>
     <t>Die Frau wurde 32 Jahre alt.</t>
   </si>
   <si>
@@ -927,6 +915,18 @@
   </si>
   <si>
     <t>&lt;u&gt;Femizid&lt;/u&gt;</t>
+  </si>
+  <si>
+    <t>factor</t>
+  </si>
+  <si>
+    <t>Die Frau überlebt. Sie ist 29 Jahre alt.</t>
+  </si>
+  <si>
+    <t>Die Frau überlebt. Sie ist 45 Jahre alt.</t>
+  </si>
+  <si>
+    <t>Die Frau überlebt. Sie ist 48 Jahre alt.</t>
   </si>
 </sst>
 </file>
@@ -1291,10 +1291,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F23"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1302,11 +1302,11 @@
     <col min="2" max="2" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="62" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="65.5703125" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1323,10 +1323,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -1342,11 +1345,14 @@
       <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>73</v>
       </c>
@@ -1362,11 +1368,14 @@
       <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>74</v>
       </c>
@@ -1382,11 +1391,14 @@
       <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="F4" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -1402,11 +1414,14 @@
       <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="F5" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>76</v>
       </c>
@@ -1422,11 +1437,14 @@
       <c r="E6" t="s">
         <v>18</v>
       </c>
-      <c r="F6" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>77</v>
       </c>
@@ -1442,11 +1460,14 @@
       <c r="E7" t="s">
         <v>20</v>
       </c>
-      <c r="F7" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>78</v>
       </c>
@@ -1462,11 +1483,14 @@
       <c r="E8" t="s">
         <v>23</v>
       </c>
-      <c r="F8" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>79</v>
       </c>
@@ -1482,11 +1506,14 @@
       <c r="E9" t="s">
         <v>26</v>
       </c>
-      <c r="F9" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>80</v>
       </c>
@@ -1502,11 +1529,14 @@
       <c r="E10" t="s">
         <v>66</v>
       </c>
-      <c r="F10" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>81</v>
       </c>
@@ -1522,11 +1552,14 @@
       <c r="E11" t="s">
         <v>20</v>
       </c>
-      <c r="F11" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>82</v>
       </c>
@@ -1542,11 +1575,14 @@
       <c r="E12" t="s">
         <v>32</v>
       </c>
-      <c r="F12" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>83</v>
       </c>
@@ -1562,11 +1598,14 @@
       <c r="E13" t="s">
         <v>69</v>
       </c>
-      <c r="F13" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>84</v>
       </c>
@@ -1582,11 +1621,14 @@
       <c r="E14" t="s">
         <v>36</v>
       </c>
-      <c r="F14" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>85</v>
       </c>
@@ -1602,11 +1644,14 @@
       <c r="E15" t="s">
         <v>38</v>
       </c>
-      <c r="F15" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>86</v>
       </c>
@@ -1622,11 +1667,14 @@
       <c r="E16" t="s">
         <v>67</v>
       </c>
-      <c r="F16" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>87</v>
       </c>
@@ -1642,11 +1690,14 @@
       <c r="E17" t="s">
         <v>8</v>
       </c>
-      <c r="F17" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>88</v>
       </c>
@@ -1662,11 +1713,14 @@
       <c r="E18" t="s">
         <v>68</v>
       </c>
-      <c r="F18" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>3</v>
+      </c>
+      <c r="G18" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>89</v>
       </c>
@@ -1674,7 +1728,7 @@
         <v>45894</v>
       </c>
       <c r="C19" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D19" t="s">
         <v>43</v>
@@ -1682,11 +1736,14 @@
       <c r="E19" t="s">
         <v>44</v>
       </c>
-      <c r="F19" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>90</v>
       </c>
@@ -1702,11 +1759,14 @@
       <c r="E20" t="s">
         <v>32</v>
       </c>
-      <c r="F20" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>91</v>
       </c>
@@ -1722,11 +1782,14 @@
       <c r="E21" t="s">
         <v>48</v>
       </c>
-      <c r="F21" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>92</v>
       </c>
@@ -1742,11 +1805,14 @@
       <c r="E22" t="s">
         <v>69</v>
       </c>
-      <c r="F22" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>93</v>
       </c>
@@ -1762,11 +1828,14 @@
       <c r="E23" t="s">
         <v>52</v>
       </c>
-      <c r="F23" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>94</v>
       </c>
@@ -1782,11 +1851,14 @@
       <c r="E24" t="s">
         <v>70</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>95</v>
       </c>
@@ -1802,11 +1874,14 @@
       <c r="E25" t="s">
         <v>56</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>96</v>
       </c>
@@ -1822,11 +1897,14 @@
       <c r="E26" t="s">
         <v>57</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>97</v>
       </c>
@@ -1842,11 +1920,14 @@
       <c r="E27" t="s">
         <v>71</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27">
+        <v>2</v>
+      </c>
+      <c r="G27" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>98</v>
       </c>
@@ -1862,11 +1943,14 @@
       <c r="E28" t="s">
         <v>58</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>99</v>
       </c>
@@ -1874,7 +1958,7 @@
         <v>45761</v>
       </c>
       <c r="C29" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D29" t="s">
         <v>59</v>
@@ -1882,11 +1966,14 @@
       <c r="E29" t="s">
         <v>60</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>100</v>
       </c>
@@ -1902,11 +1989,14 @@
       <c r="E30" t="s">
         <v>62</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>101</v>
       </c>
@@ -1922,7 +2012,10 @@
       <c r="E31" t="s">
         <v>65</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1934,10 +2027,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0ACE054-CF54-402D-BA14-1540848E52E5}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1945,11 +2038,12 @@
     <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="77.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.28515625" customWidth="1"/>
+    <col min="6" max="6" width="39" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1966,10 +2060,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>102</v>
       </c>
@@ -1985,11 +2082,14 @@
       <c r="E2" t="s">
         <v>152</v>
       </c>
-      <c r="F2" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>103</v>
       </c>
@@ -2005,11 +2105,14 @@
       <c r="E3" t="s">
         <v>151</v>
       </c>
-      <c r="F3" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>104</v>
       </c>
@@ -2025,11 +2128,14 @@
       <c r="E4" t="s">
         <v>227</v>
       </c>
-      <c r="F4" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>105</v>
       </c>
@@ -2045,11 +2151,14 @@
       <c r="E5" t="s">
         <v>148</v>
       </c>
-      <c r="F5" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>106</v>
       </c>
@@ -2065,11 +2174,14 @@
       <c r="E6" t="s">
         <v>18</v>
       </c>
-      <c r="F6" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>107</v>
       </c>
@@ -2085,11 +2197,14 @@
       <c r="E7" t="s">
         <v>150</v>
       </c>
-      <c r="F7" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>108</v>
       </c>
@@ -2105,11 +2220,14 @@
       <c r="E8" t="s">
         <v>69</v>
       </c>
-      <c r="F8" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>109</v>
       </c>
@@ -2125,11 +2243,14 @@
       <c r="E9" t="s">
         <v>48</v>
       </c>
-      <c r="F9" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>110</v>
       </c>
@@ -2145,11 +2266,14 @@
       <c r="E10" t="s">
         <v>69</v>
       </c>
-      <c r="F10" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>111</v>
       </c>
@@ -2165,11 +2289,14 @@
       <c r="E11" t="s">
         <v>26</v>
       </c>
-      <c r="F11" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>112</v>
       </c>
@@ -2185,11 +2312,14 @@
       <c r="E12" t="s">
         <v>149</v>
       </c>
-      <c r="F12" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>113</v>
       </c>
@@ -2205,11 +2335,14 @@
       <c r="E13" t="s">
         <v>148</v>
       </c>
-      <c r="F13" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>114</v>
       </c>
@@ -2225,11 +2358,14 @@
       <c r="E14" t="s">
         <v>147</v>
       </c>
-      <c r="F14" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>115</v>
       </c>
@@ -2245,11 +2381,14 @@
       <c r="E15" t="s">
         <v>18</v>
       </c>
-      <c r="F15" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>116</v>
       </c>
@@ -2265,11 +2404,14 @@
       <c r="E16" t="s">
         <v>146</v>
       </c>
-      <c r="F16" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>117</v>
       </c>
@@ -2285,11 +2427,14 @@
       <c r="E17" t="s">
         <v>143</v>
       </c>
-      <c r="F17" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>118</v>
       </c>
@@ -2305,11 +2450,14 @@
       <c r="E18" t="s">
         <v>145</v>
       </c>
-      <c r="F18" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="G18" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>119</v>
       </c>
@@ -2325,11 +2473,14 @@
       <c r="E19" t="s">
         <v>52</v>
       </c>
-      <c r="F19" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>120</v>
       </c>
@@ -2345,11 +2496,14 @@
       <c r="E20" t="s">
         <v>144</v>
       </c>
-      <c r="F20" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>121</v>
       </c>
@@ -2365,11 +2519,14 @@
       <c r="E21" t="s">
         <v>143</v>
       </c>
-      <c r="F21" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>122</v>
       </c>
@@ -2385,7 +2542,10 @@
       <c r="E22" t="s">
         <v>142</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2396,10 +2556,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB42D47A-EC97-4604-B6C9-50F5C4DCAF25}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2409,10 +2569,11 @@
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="54" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2429,10 +2590,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>153</v>
       </c>
@@ -2448,11 +2612,14 @@
       <c r="E2" t="s">
         <v>32</v>
       </c>
-      <c r="F2" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>154</v>
       </c>
@@ -2468,11 +2635,14 @@
       <c r="E3" t="s">
         <v>205</v>
       </c>
-      <c r="F3" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>155</v>
       </c>
@@ -2488,11 +2658,14 @@
       <c r="E4" t="s">
         <v>204</v>
       </c>
-      <c r="F4" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>156</v>
       </c>
@@ -2508,11 +2681,14 @@
       <c r="E5" t="s">
         <v>69</v>
       </c>
-      <c r="F5" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>157</v>
       </c>
@@ -2528,11 +2704,14 @@
       <c r="E6" t="s">
         <v>152</v>
       </c>
-      <c r="F6" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>158</v>
       </c>
@@ -2548,11 +2727,14 @@
       <c r="E7" t="s">
         <v>69</v>
       </c>
-      <c r="F7" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>159</v>
       </c>
@@ -2568,11 +2750,14 @@
       <c r="E8" t="s">
         <v>203</v>
       </c>
-      <c r="F8" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>160</v>
       </c>
@@ -2588,11 +2773,14 @@
       <c r="E9" t="s">
         <v>202</v>
       </c>
-      <c r="F9" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>161</v>
       </c>
@@ -2608,11 +2796,14 @@
       <c r="E10" t="s">
         <v>201</v>
       </c>
-      <c r="F10" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>162</v>
       </c>
@@ -2628,11 +2819,14 @@
       <c r="E11" t="s">
         <v>48</v>
       </c>
-      <c r="F11" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>163</v>
       </c>
@@ -2648,11 +2842,14 @@
       <c r="E12" t="s">
         <v>200</v>
       </c>
-      <c r="F12" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>164</v>
       </c>
@@ -2668,11 +2865,14 @@
       <c r="E13" t="s">
         <v>199</v>
       </c>
-      <c r="F13" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>165</v>
       </c>
@@ -2688,11 +2888,14 @@
       <c r="E14" t="s">
         <v>152</v>
       </c>
-      <c r="F14" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>166</v>
       </c>
@@ -2708,11 +2911,14 @@
       <c r="E15" t="s">
         <v>32</v>
       </c>
-      <c r="F15" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>167</v>
       </c>
@@ -2728,11 +2934,14 @@
       <c r="E16" t="s">
         <v>8</v>
       </c>
-      <c r="F16" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>168</v>
       </c>
@@ -2748,11 +2957,14 @@
       <c r="E17" t="s">
         <v>8</v>
       </c>
-      <c r="F17" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>169</v>
       </c>
@@ -2768,11 +2980,14 @@
       <c r="E18" t="s">
         <v>198</v>
       </c>
-      <c r="F18" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>170</v>
       </c>
@@ -2788,11 +3003,14 @@
       <c r="E19" t="s">
         <v>197</v>
       </c>
-      <c r="F19" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>171</v>
       </c>
@@ -2808,11 +3026,14 @@
       <c r="E20" t="s">
         <v>195</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>172</v>
       </c>
@@ -2828,11 +3049,14 @@
       <c r="E21" t="s">
         <v>194</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>173</v>
       </c>
@@ -2848,11 +3072,14 @@
       <c r="E22" t="s">
         <v>196</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>174</v>
       </c>
@@ -2868,7 +3095,10 @@
       <c r="E23" t="s">
         <v>193</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2880,10 +3110,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{504B19E9-6DB8-44C6-AC2E-AFFBAC43FF71}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2892,10 +3122,11 @@
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2912,10 +3143,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>206</v>
       </c>
@@ -2931,11 +3165,14 @@
       <c r="E2" t="s">
         <v>200</v>
       </c>
-      <c r="F2" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>207</v>
       </c>
@@ -2946,16 +3183,19 @@
         <v>141</v>
       </c>
       <c r="D3" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E3" t="s">
-        <v>248</v>
-      </c>
-      <c r="F3" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>208</v>
       </c>
@@ -2963,19 +3203,22 @@
         <v>44632</v>
       </c>
       <c r="C4" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D4" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E4" t="s">
-        <v>253</v>
-      </c>
-      <c r="F4" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>209</v>
       </c>
@@ -2986,16 +3229,19 @@
         <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E5" t="s">
-        <v>251</v>
-      </c>
-      <c r="F5" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>210</v>
       </c>
@@ -3006,16 +3252,19 @@
         <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E6" t="s">
-        <v>252</v>
-      </c>
-      <c r="F6" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>211</v>
       </c>
@@ -3026,16 +3275,19 @@
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E7" t="s">
         <v>143</v>
       </c>
-      <c r="F7" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>212</v>
       </c>
@@ -3046,16 +3298,19 @@
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E8" t="s">
         <v>69</v>
       </c>
-      <c r="F8" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>213</v>
       </c>
@@ -3069,13 +3324,16 @@
         <v>189</v>
       </c>
       <c r="E9" t="s">
-        <v>249</v>
-      </c>
-      <c r="F9" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>214</v>
       </c>
@@ -3086,16 +3344,19 @@
         <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E10" t="s">
-        <v>250</v>
-      </c>
-      <c r="F10" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>215</v>
       </c>
@@ -3111,11 +3372,14 @@
       <c r="E11" t="s">
         <v>11</v>
       </c>
-      <c r="F11" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>216</v>
       </c>
@@ -3126,16 +3390,19 @@
         <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E12" t="s">
         <v>200</v>
       </c>
-      <c r="F12" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>217</v>
       </c>
@@ -3143,19 +3410,22 @@
         <v>44818</v>
       </c>
       <c r="C13" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D13" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E13" t="s">
         <v>151</v>
       </c>
-      <c r="F13" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>218</v>
       </c>
@@ -3166,16 +3436,19 @@
         <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E14" t="s">
-        <v>249</v>
-      </c>
-      <c r="F14" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>219</v>
       </c>
@@ -3189,13 +3462,16 @@
         <v>136</v>
       </c>
       <c r="E15" t="s">
-        <v>248</v>
-      </c>
-      <c r="F15" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>220</v>
       </c>
@@ -3206,16 +3482,19 @@
         <v>22</v>
       </c>
       <c r="D16" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E16" t="s">
         <v>18</v>
       </c>
-      <c r="F16" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>221</v>
       </c>
@@ -3226,16 +3505,19 @@
         <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E17" t="s">
         <v>146</v>
       </c>
-      <c r="F17" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>222</v>
       </c>
@@ -3251,11 +3533,14 @@
       <c r="E18" t="s">
         <v>231</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>223</v>
       </c>
@@ -3271,11 +3556,14 @@
       <c r="E19" t="s">
         <v>232</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>224</v>
       </c>
@@ -3289,13 +3577,16 @@
         <v>230</v>
       </c>
       <c r="E20" t="s">
-        <v>233</v>
-      </c>
-      <c r="F20" t="s">
+        <v>298</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>225</v>
       </c>
@@ -3309,13 +3600,16 @@
         <v>229</v>
       </c>
       <c r="E21" t="s">
-        <v>234</v>
-      </c>
-      <c r="F21" t="s">
+        <v>299</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>226</v>
       </c>
@@ -3329,9 +3623,12 @@
         <v>228</v>
       </c>
       <c r="E22" t="s">
-        <v>235</v>
-      </c>
-      <c r="F22" t="s">
+        <v>300</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
         <v>54</v>
       </c>
     </row>
@@ -3342,10 +3639,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D886333-151F-4F81-A8CC-E4D884E81DCA}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3354,11 +3651,12 @@
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="112.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.85546875" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3375,12 +3673,15 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B2" s="3">
         <v>43831</v>
@@ -3394,13 +3695,16 @@
       <c r="E2" t="s">
         <v>18</v>
       </c>
-      <c r="F2" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B3" s="3">
         <v>43856</v>
@@ -3414,13 +3718,16 @@
       <c r="E3" t="s">
         <v>26</v>
       </c>
-      <c r="F3" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B4" s="3">
         <v>43893</v>
@@ -3429,18 +3736,21 @@
         <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="F4" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B5" s="3">
         <v>43908</v>
@@ -3449,18 +3759,21 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
       </c>
-      <c r="F5" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B6" s="3">
         <v>43923</v>
@@ -3472,15 +3785,18 @@
         <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>298</v>
-      </c>
-      <c r="F6" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B7" s="3">
         <v>43936</v>
@@ -3489,18 +3805,21 @@
         <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="E7" t="s">
-        <v>297</v>
-      </c>
-      <c r="F7" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>293</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B8" s="3">
         <v>43967</v>
@@ -3509,18 +3828,21 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="E8" t="s">
         <v>8</v>
       </c>
-      <c r="F8" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B9" s="3">
         <v>43968</v>
@@ -3529,18 +3851,21 @@
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="E9" t="s">
         <v>32</v>
       </c>
-      <c r="F9" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B10" s="3">
         <v>43996</v>
@@ -3554,13 +3879,16 @@
       <c r="E10" t="s">
         <v>32</v>
       </c>
-      <c r="F10" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B11" s="3">
         <v>44002</v>
@@ -3572,15 +3900,18 @@
         <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>296</v>
-      </c>
-      <c r="F11" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B12" s="3">
         <v>44067</v>
@@ -3589,38 +3920,44 @@
         <v>50</v>
       </c>
       <c r="D12" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="E12" t="s">
         <v>201</v>
       </c>
-      <c r="F12" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B13" s="3">
         <v>44076</v>
       </c>
       <c r="C13" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D13" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="E13" t="s">
         <v>152</v>
       </c>
-      <c r="F13" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B14" s="3">
         <v>44095</v>
@@ -3629,18 +3966,21 @@
         <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E14" t="s">
         <v>48</v>
       </c>
-      <c r="F14" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B15" s="3">
         <v>44139</v>
@@ -3649,18 +3989,21 @@
         <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="E15" t="s">
         <v>69</v>
       </c>
-      <c r="F15" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B16" s="3">
         <v>44190</v>
@@ -3669,18 +4012,21 @@
         <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="E16" t="s">
         <v>69</v>
       </c>
-      <c r="F16" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B17" s="3">
         <v>44195</v>
@@ -3689,38 +4035,44 @@
         <v>50</v>
       </c>
       <c r="D17" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="E17" t="s">
-        <v>295</v>
-      </c>
-      <c r="F17" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>291</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B18" s="3">
         <v>44061</v>
       </c>
       <c r="C18" t="s">
+        <v>275</v>
+      </c>
+      <c r="D18" t="s">
+        <v>274</v>
+      </c>
+      <c r="E18" t="s">
         <v>279</v>
       </c>
-      <c r="D18" t="s">
-        <v>278</v>
-      </c>
-      <c r="E18" t="s">
-        <v>283</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B19" s="3">
         <v>44079</v>
@@ -3729,18 +4081,21 @@
         <v>25</v>
       </c>
       <c r="D19" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="E19" t="s">
-        <v>282</v>
-      </c>
-      <c r="F19" t="s">
+        <v>278</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B20" s="3">
         <v>44107</v>
@@ -3749,18 +4104,21 @@
         <v>25</v>
       </c>
       <c r="D20" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="E20" t="s">
-        <v>281</v>
-      </c>
-      <c r="F20" t="s">
+        <v>277</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="B21" s="4">
         <v>44133</v>
@@ -3769,18 +4127,21 @@
         <v>50</v>
       </c>
       <c r="D21" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="E21" t="s">
         <v>195</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B22" s="3">
         <v>44164</v>
@@ -3789,12 +4150,15 @@
         <v>17</v>
       </c>
       <c r="D22" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="E22" t="s">
-        <v>280</v>
-      </c>
-      <c r="F22" t="s">
+        <v>276</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>